<commit_message>
Actualizar cabanas y calendario
Se arreglo el bug de actualizacion en cabanas.

Se agrego la funcion de actualizar al crud de calendario.
</commit_message>
<xml_diff>
--- a/static/reportes/reporte No. 1.xlsx
+++ b/static/reportes/reporte No. 1.xlsx
@@ -417,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -464,31 +464,31 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Erick Jonathan </t>
+          <t>Prueba</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Bautista</t>
+          <t>Prueba</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Perez</t>
+          <t>Prueba</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>f4k3r</t>
+          <t>Prueba</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>erick.bautista57@hotmail.com</t>
+          <t>aaaa@gmail.com</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -499,31 +499,31 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Ramiro de Jesús</t>
+          <t>Yomer</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Hernández</t>
+          <t>asies</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t xml:space="preserve">Bernabé </t>
+          <t>asies</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>nalgoncito</t>
+          <t>asies</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>ramironalgon@gmail.com</t>
+          <t>asies@gmail.com</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -534,31 +534,31 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>José Manuel</t>
+          <t>Ramiro</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Jimeno </t>
+          <t>De Jesus</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t xml:space="preserve">Islas </t>
+          <t>Hernandez</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t xml:space="preserve">ChemigodElite </t>
+          <t>RamboBernabe</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>elitefortgod@gmail.com</t>
+          <t>ramironchis@gmail.com</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -569,31 +569,31 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Gilberto</t>
+          <t>Gilberta</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
+          <t>Olivares</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
           <t>Cruz</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Olivares</t>
-        </is>
-      </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>C0Gil</t>
+          <t>ElGil</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>gil123@gmail.com</t>
+          <t>gilimemo@gmail.com</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -604,11 +604,11 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Luis Eduardo</t>
+          <t xml:space="preserve">Erick Jonathan </t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -623,50 +623,330 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>elsanto</t>
+          <t>f4k3r</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>luisbautista@example.com</t>
+          <t>erick.bautista57@hotmail.com</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Supervisor</t>
+          <t>Administrador</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Ramiro de Jesús</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Hernández</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Bernabé </t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>nalgoncito</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>ramironalgon@gmail.com</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Administrador</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>José Manuel</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Jimeno </t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Islas </t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ChemigodElite </t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>elitefortgod@gmail.com</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Administrador</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>4</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Gilberto</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Cruz</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Olivares</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>C0Gil</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>gil123@gmail.com</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Administrador</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>17</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Luis2</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Lopez2</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Delgado2</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Cerre2</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>luis2@gmail.com</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Supervisor</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>16</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Luis</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Lopez</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Delgado</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Cerre</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>luis@gmail.com</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Supervisor</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>15</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Teofilito</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Hernandez</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Bernabe</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Teo</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>teo@gmail.com</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Supervisor</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>13</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Misterbist</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Señor</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Bestia</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>MrB</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>pokimike@gmail.com</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Supervisor</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>8</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Luis Eduardo</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Bautista</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Perez</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>elsanto</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>luisbautista@example.com</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Supervisor</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
         <v>5</v>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="B15" t="inlineStr">
         <is>
           <t>Juan Miguel</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="C15" t="inlineStr">
         <is>
           <t>Sanchez</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="D15" t="inlineStr">
         <is>
           <t>Aguilar</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="E15" t="inlineStr">
         <is>
           <t>pokimike</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="F15" t="inlineStr">
         <is>
           <t>pokimike@gmail.com</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
+      <c r="G15" t="inlineStr">
         <is>
           <t>Supervisor</t>
         </is>

</xml_diff>